<commit_message>
220831 보충 project update
</commit_message>
<xml_diff>
--- a/김성근_SQL/항공table.xlsx
+++ b/김성근_SQL/항공table.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="25427"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\ss\SQL_project\김성근_SQL\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\Documents\GitHub\SQL_project\김성근_SQL\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD923B33-F574-4C37-95A4-869CFD2EF57B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="45" yWindow="0" windowWidth="14520" windowHeight="15075"/>
+    <workbookView xWindow="45" yWindow="0" windowWidth="14520" windowHeight="15075" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -221,7 +222,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -648,11 +649,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:L28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H20" sqref="H20"/>
+      <selection activeCell="B9" sqref="B9:H11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -1018,7 +1019,7 @@
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <hyperlinks>
-    <hyperlink ref="L1" r:id="rId1"/>
+    <hyperlink ref="L1" r:id="rId1" xr:uid="{00000000-0004-0000-0000-000000000000}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId2"/>

</xml_diff>